<commit_message>
creating google forms using data from excel in uipath
</commit_message>
<xml_diff>
--- a/RPA_Project_Fill_Optionale/SortareRezultateForms/raspunsuri.xlsx
+++ b/RPA_Project_Fill_Optionale/SortareRezultateForms/raspunsuri.xlsx
@@ -8,22 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\my_github\uipath\proiect_rpa\RPA_Project_Fill_Optionale\SortareRezultateForms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618BA142-5000-4611-A285-AB7AACF306B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD03F9EC-C7E9-4698-91D2-0F6AC46298C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Răspunsuri la formular" sheetId="1" r:id="rId1"/>
     <sheet name="Date studenti" sheetId="3" r:id="rId2"/>
     <sheet name="Repartizare" sheetId="2" r:id="rId3"/>
-    <sheet name="Discipline" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
   <si>
     <t>Marcaj de timp</t>
   </si>
@@ -236,18 +235,6 @@
   </si>
   <si>
     <t>Introducere in neurotehnologii</t>
-  </si>
-  <si>
-    <t>Sem 1, prima opțională</t>
-  </si>
-  <si>
-    <t>Sem 1, a doua opțională</t>
-  </si>
-  <si>
-    <t>Sem 2, prima opțională</t>
-  </si>
-  <si>
-    <t>Sem 2, a-2-a opțională</t>
   </si>
 </sst>
 </file>
@@ -560,31 +547,31 @@
   </sheetPr>
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="52" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="47.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="67.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="67.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="53.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="46.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="21" width="18.85546875" customWidth="1"/>
+    <col min="6" max="7" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="67.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="67.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="21" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -634,7 +621,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
@@ -684,7 +671,7 @@
         <v>9.4290000000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -734,7 +721,7 @@
         <v>9.3859999999999992</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -784,7 +771,7 @@
         <v>9.2240000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -834,7 +821,7 @@
         <v>8.9659999999999993</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
@@ -884,7 +871,7 @@
         <v>8.5579999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -934,7 +921,7 @@
         <v>8.3089999999999993</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -984,7 +971,7 @@
         <v>8.0630000000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -1034,7 +1021,7 @@
         <v>8.0570000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
@@ -1084,7 +1071,7 @@
         <v>7.915</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -1134,7 +1121,7 @@
         <v>7.9059999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
@@ -1184,7 +1171,7 @@
         <v>7.508</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -1234,7 +1221,7 @@
         <v>7.2149999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
@@ -1284,7 +1271,7 @@
         <v>7.1669999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1334,7 +1321,7 @@
         <v>7.1539999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>34</v>
       </c>
@@ -1384,7 +1371,7 @@
         <v>7.0949999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -1434,7 +1421,7 @@
         <v>6.7789999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
@@ -1484,7 +1471,7 @@
         <v>6.3630000000000004</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
@@ -1534,7 +1521,7 @@
         <v>6.0860000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
@@ -1584,7 +1571,7 @@
         <v>5.6509999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
@@ -1651,13 +1638,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -1665,164 +1652,164 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
       <c r="B2">
-        <v>9.4290000000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>8.6910000000000007</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3">
+        <v>8.2509999999999994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4">
+        <v>8.3140000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>9.2189999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6">
+        <v>6.9809999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7">
+        <v>9.0690000000000008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8">
+        <v>7.407</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9">
+        <v>8.8879999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10">
+        <v>7.7469999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11">
+        <v>6.3819999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12">
+        <v>5.6749999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13">
+        <v>5.0179999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14">
+        <v>5.7960000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15">
+        <v>8.8800000000000008</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16">
+        <v>7.1669999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18">
+        <v>7.6239999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19">
+        <v>8.1069999999999993</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>35</v>
       </c>
-      <c r="B3">
-        <v>5.0170000000000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4">
-        <v>8.5579999999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5">
-        <v>7.915</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6">
-        <v>7.508</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7">
-        <v>7.1539999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8">
-        <v>6.7789999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9">
-        <v>9.2240000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10">
-        <v>7.1669999999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11">
-        <v>8.3089999999999993</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12">
-        <v>7.2149999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13">
-        <v>6.3630000000000004</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14">
-        <v>8.0570000000000004</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15">
-        <v>9.3859999999999992</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16">
-        <v>5.6509999999999998</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17">
-        <v>8.9659999999999993</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18">
-        <v>7.9059999999999997</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19">
-        <v>7.0949999999999998</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20">
-        <v>6.0860000000000003</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>39</v>
-      </c>
       <c r="B21">
-        <v>8.0630000000000006</v>
+        <v>9.8889999999999993</v>
       </c>
     </row>
   </sheetData>
@@ -1834,27 +1821,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:XFD19"/>
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="46.44140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="46" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -1893,99 +1880,6 @@
       </c>
       <c r="P1" t="s">
         <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A09AC581-B567-454F-9B9E-32FD584D5E71}">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="46" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C6" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>